<commit_message>
first version of database creation
also update disease search terms cols
</commit_message>
<xml_diff>
--- a/raw_data/manual_input/disease_search_terms.xlsx
+++ b/raw_data/manual_input/disease_search_terms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/kristina_thompson_wur_nl/Documents/Dutch infectious disease database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikj\surfdrive\SoDa\projects\disease_database\raw_data\manual_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C6D4D50-8A84-423B-9EAE-171F495A64FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E651C320-8FEF-4A99-BB2E-D940002D2400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{02459005-B8AB-421A-9E44-69286374966E}"/>
+    <workbookView xWindow="5700" yWindow="2700" windowWidth="21480" windowHeight="12630" xr2:uid="{02459005-B8AB-421A-9E44-69286374966E}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t xml:space="preserve">Food- and water-borne infectious diseases </t>
   </si>
@@ -78,9 +78,6 @@
     <t>Acute respiratory disease (including influenza)</t>
   </si>
   <si>
-    <t>Regex search</t>
-  </si>
-  <si>
     <t>Airborne infectious diseases</t>
   </si>
   <si>
@@ -136,6 +133,54 @@
   </si>
   <si>
     <t>kraam.?koorts|kraam.?vrouwen.?koorts</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Typhus</t>
+  </si>
+  <si>
+    <t>Dysentery</t>
+  </si>
+  <si>
+    <t>Cholera</t>
+  </si>
+  <si>
+    <t>Malaria</t>
+  </si>
+  <si>
+    <t>ScarletFever</t>
+  </si>
+  <si>
+    <t>Tuberculosis</t>
+  </si>
+  <si>
+    <t>Diphteria</t>
+  </si>
+  <si>
+    <t>WhoopingCouvh</t>
+  </si>
+  <si>
+    <t>Influenza</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Brain</t>
+  </si>
+  <si>
+    <t>PuerperalFever</t>
+  </si>
+  <si>
+    <t>Regex</t>
   </si>
 </sst>
 </file>
@@ -198,9 +243,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -238,7 +283,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -344,7 +389,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -486,7 +531,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -494,163 +539,252 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AAA744-FA2D-437D-BC13-23A6A0E9F475}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="83.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -666,21 +800,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update readme, big updates for main and postproc
- better input data
- renamed database_flat
- more complex query with optional proximity
- renamed "municipality" to "location"
</commit_message>
<xml_diff>
--- a/raw_data/manual_input/disease_search_terms.xlsx
+++ b/raw_data/manual_input/disease_search_terms.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikj\surfdrive\SoDa\projects\disease_database\raw_data\manual_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E651C320-8FEF-4A99-BB2E-D940002D2400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFDCD17-FE6A-4E6E-8F7E-AFE39ABECCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="2700" windowWidth="21480" windowHeight="12630" xr2:uid="{02459005-B8AB-421A-9E44-69286374966E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{02459005-B8AB-421A-9E44-69286374966E}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="3" r:id="rId1"/>
     <sheet name="Notes on sources" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$A$1:$D$11</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t xml:space="preserve">Food- and water-borne infectious diseases </t>
   </si>
@@ -72,18 +75,12 @@
     <t>Croup; Diphtheria</t>
   </si>
   <si>
-    <t>Whooping cough</t>
-  </si>
-  <si>
     <t>Acute respiratory disease (including influenza)</t>
   </si>
   <si>
     <t>Airborne infectious diseases</t>
   </si>
   <si>
-    <t>puerperal fever</t>
-  </si>
-  <si>
     <t>Other infectious diseases (mixed aetiology)</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>Source: Boomen, N. van den (ed.), Born close to death. Region, Roman Catholicism and infant mortality in the Netherlands, 1875-1899, pp. 119-156</t>
   </si>
   <si>
-    <t>Brain diseases (insanity; diseases of the spinal cord; paralysis; syphilis; convulsions; trismus; epilepsy)</t>
-  </si>
-  <si>
     <t>Malaria (including: intermittent fever; pernicious fever)</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
     <t>malaria|moeras.?koorts|polder.?koorts</t>
   </si>
   <si>
-    <t>kraam.?koorts|kraam.?vrouwen.?koorts</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
@@ -159,25 +150,7 @@
     <t>Diphteria</t>
   </si>
   <si>
-    <t>WhoopingCouvh</t>
-  </si>
-  <si>
     <t>Influenza</t>
-  </si>
-  <si>
-    <t>Include</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Brain</t>
-  </si>
-  <si>
-    <t>PuerperalFever</t>
   </si>
   <si>
     <t>Regex</t>
@@ -196,18 +169,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -222,9 +189,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,255 +505,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AAA744-FA2D-437D-BC13-23A6A0E9F475}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="83.42578125" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.42578125" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
       <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
       <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:D11" xr:uid="{76AAA744-FA2D-437D-BC13-23A6A0E9F475}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -804,17 +691,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add word boundaries to disease search terms
</commit_message>
<xml_diff>
--- a/raw_data/manual_input/disease_search_terms.xlsx
+++ b/raw_data/manual_input/disease_search_terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikj\surfdrive\SoDa\projects\disease_database\raw_data\manual_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFDCD17-FE6A-4E6E-8F7E-AFE39ABECCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90CD9B8-F236-48C7-B84D-852DF0687BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{02459005-B8AB-421A-9E44-69286374966E}"/>
+    <workbookView xWindow="4965" yWindow="5078" windowWidth="21600" windowHeight="12682" xr2:uid="{02459005-B8AB-421A-9E44-69286374966E}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="3" r:id="rId1"/>
@@ -96,36 +96,6 @@
     <t>Malaria (including: intermittent fever; pernicious fever)</t>
   </si>
   <si>
-    <t>ty(ph|f)(us|euz.)|febris.?typhoidea|kwaadaardige.*koorts</t>
-  </si>
-  <si>
-    <t>diarrhoea|dysenter.*|rood.?loop|buik.?loop|bloed.?gang</t>
-  </si>
-  <si>
-    <t>choler.*|krim.?koorts</t>
-  </si>
-  <si>
-    <t>pokken|variola</t>
-  </si>
-  <si>
-    <t>rood.?vonk|scarlatina|scharlaken.?koorts</t>
-  </si>
-  <si>
-    <t>mazelen|rood.?ziekte|rubeola|rubella</t>
-  </si>
-  <si>
-    <t>tering|verteringsziekte</t>
-  </si>
-  <si>
-    <t>(c|k)roup|angina.?diphtheri.*|diphtheri.*|difteritis</t>
-  </si>
-  <si>
-    <t>griep|influenza</t>
-  </si>
-  <si>
-    <t>malaria|moeras.?koorts|polder.?koorts</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
@@ -154,6 +124,36 @@
   </si>
   <si>
     <t>Regex</t>
+  </si>
+  <si>
+    <t>(?:[^a-zA-Z]|\b)(ty(ph|f)(us|euz.)|febris.?typhoidea|kwaadaardige.*koorts)(?:[^a-zA-Z]|\b)</t>
+  </si>
+  <si>
+    <t>(?:[^a-zA-Z]|\b)(diarrhoea|dysenter.*|rood.?loop|buik.?loop|bloed.?gang)(?:[^a-zA-Z]|\b)</t>
+  </si>
+  <si>
+    <t>(?:[^a-zA-Z]|\b)(choler.*|krim.?koorts)(?:[^a-zA-Z]|\b)</t>
+  </si>
+  <si>
+    <t>(?:[^a-zA-Z]|\b)(pokken|variola)(?:[^a-zA-Z]|\b)</t>
+  </si>
+  <si>
+    <t>(?:[^a-zA-Z]|\b)(rood.?vonk|scarlatina|scharlaken.?koorts)(?:[^a-zA-Z]|\b)</t>
+  </si>
+  <si>
+    <t>(?:[^a-zA-Z]|\b)(mazelen|rood.?ziekte|rubeola|rubella)(?:[^a-zA-Z]|\b)</t>
+  </si>
+  <si>
+    <t>(?:[^a-zA-Z]|\b)(tering|verteringsziekte)(?:[^a-zA-Z]|\b)</t>
+  </si>
+  <si>
+    <t>(?:[^a-zA-Z]|\b)((c|k)roup|angina.?diphtheri.*|diphtheri.*|difteritis)(?:[^a-zA-Z]|\b)</t>
+  </si>
+  <si>
+    <t>(?:[^a-zA-Z]|\b)(griep|influenza)(?:[^a-zA-Z]|\b)</t>
+  </si>
+  <si>
+    <t>(?:[^a-zA-Z]|\b)(malaria|moeras.?koorts|polder.?koorts)(?:[^a-zA-Z]|\b)</t>
   </si>
 </sst>
 </file>
@@ -507,21 +507,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AAA744-FA2D-437D-BC13-23A6A0E9F475}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.3984375" customWidth="1"/>
+    <col min="3" max="3" width="40.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -530,12 +530,12 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -544,12 +544,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -558,12 +558,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -572,10 +572,10 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -586,12 +586,12 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -600,10 +600,10 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -614,12 +614,12 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -628,12 +628,12 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -642,12 +642,12 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -656,12 +656,12 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -670,7 +670,7 @@
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -687,19 +687,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>16</v>
       </c>

</xml_diff>